<commit_message>
dded new guard panel, new admin rights updated security and many other features
</commit_message>
<xml_diff>
--- a/backend/visitors.xlsx
+++ b/backend/visitors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -47,6 +47,39 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751387857/visitors/zteo6zz2hxch0vdouhmc.jpg</t>
+  </si>
+  <si>
+    <t>dcsdc</t>
+  </si>
+  <si>
+    <t>dfvdfv</t>
+  </si>
+  <si>
+    <t>fvdfa</t>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>2/7/2025, 9:21:18 pm</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751471478/visitors/iexcozqvsik1snensf9n.jpg</t>
+  </si>
+  <si>
+    <t>fefaef</t>
+  </si>
+  <si>
+    <t>gsergrse</t>
+  </si>
+  <si>
+    <t>gtsrtg</t>
+  </si>
+  <si>
+    <t>2/7/2025, 9:28:47 pm</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751471927/visitors/q1cx4nvgvwz4asjemjf1.jpg</t>
   </si>
 </sst>
 </file>
@@ -423,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -474,6 +507,46 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
added condition for 10 digit phone number
</commit_message>
<xml_diff>
--- a/backend/visitors.xlsx
+++ b/backend/visitors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -47,39 +47,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751387857/visitors/zteo6zz2hxch0vdouhmc.jpg</t>
-  </si>
-  <si>
-    <t>dcsdc</t>
-  </si>
-  <si>
-    <t>dfvdfv</t>
-  </si>
-  <si>
-    <t>fvdfa</t>
-  </si>
-  <si>
-    <t>approved</t>
-  </si>
-  <si>
-    <t>2/7/2025, 9:21:18 pm</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751471478/visitors/iexcozqvsik1snensf9n.jpg</t>
-  </si>
-  <si>
-    <t>fefaef</t>
-  </si>
-  <si>
-    <t>gsergrse</t>
-  </si>
-  <si>
-    <t>gtsrtg</t>
-  </si>
-  <si>
-    <t>2/7/2025, 9:28:47 pm</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751471927/visitors/q1cx4nvgvwz4asjemjf1.jpg</t>
   </si>
 </sst>
 </file>
@@ -456,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -507,46 +474,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
🔧 Implemented Push Notification Support + UI/Backend Enhancements
</commit_message>
<xml_diff>
--- a/backend/visitors.xlsx
+++ b/backend/visitors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -31,33 +31,12 @@
     <t>Photo URL</t>
   </si>
   <si>
-    <t>Pancholi dn</t>
-  </si>
-  <si>
-    <t>9424812728</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>rejected</t>
-  </si>
-  <si>
-    <t>1/7/2025, 10:07:38 pm</t>
-  </si>
-  <si>
-    <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751387857/visitors/zteo6zz2hxch0vdouhmc.jpg</t>
-  </si>
-  <si>
     <t>Harsh</t>
   </si>
   <si>
     <t>1234567890</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>approved</t>
   </si>
   <si>
@@ -65,6 +44,27 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751632271/visitors/gdet8s6acynxjzp5tibe.jpg</t>
+  </si>
+  <si>
+    <t>2134224231</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>5/7/2025, 12:37:40 pm</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751699260/visitors/s8lx4buuoboaabtz39lh.jpg</t>
+  </si>
+  <si>
+    <t>3458365863</t>
+  </si>
+  <si>
+    <t>5/7/2025, 12:40:26 pm</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/drdw2abup/image/upload/v1751699426/visitors/y2lqbutnk4n2xgjvbtmk.jpg</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -479,36 +479,47 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>